<commit_message>
edits and added code crosswalk file
</commit_message>
<xml_diff>
--- a/CMECS_Catalog_v1.1.1/SC_Comparison_Tables_v1.0.0-v1.1.0.xlsx
+++ b/CMECS_Catalog_v1.1.1/SC_Comparison_Tables_v1.0.0-v1.1.0.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kate.rose\Documents\CMECS_1.1.1\CMECS_Catalog_v1.1.1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C657322F-FF5B-4686-B37A-C36EA1AB8B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886B5130-32BE-4548-9E7D-9EEB7E77E89A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24870" windowHeight="10980" xr2:uid="{11850F52-B992-4978-99CC-358F33DA057C}"/>
   </bookViews>
@@ -1906,6 +1901,93 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1913,15 +1995,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1935,84 +2008,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2354,20 +2349,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="H1" s="81" t="s">
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="H1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
     </row>
     <row r="2" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2413,10 +2408,10 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="96" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2425,10 +2420,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="87" t="s">
+      <c r="H3" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="122" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="10" t="s">
@@ -2447,16 +2442,16 @@
     </row>
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="86"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="15"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="90"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="122"/>
       <c r="J4" s="16" t="s">
         <v>12</v>
       </c>
@@ -2473,14 +2468,14 @@
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="83"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="17"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19"/>
       <c r="F5" s="20"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="91"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="123"/>
       <c r="J5" s="21" t="s">
         <v>13</v>
       </c>
@@ -2497,28 +2492,28 @@
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="92" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="85" t="s">
+      <c r="D6" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="79" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="95" t="s">
+      <c r="H6" s="120"/>
+      <c r="I6" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="92" t="s">
+      <c r="J6" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="85" t="s">
+      <c r="K6" s="96" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="25" t="s">
@@ -2535,18 +2530,18 @@
     </row>
     <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
       <c r="F7" s="24" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="86"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="82"/>
       <c r="L7" s="26" t="s">
         <v>21</v>
       </c>
@@ -2561,18 +2556,18 @@
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="92" t="s">
+      <c r="H8" s="120"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="79" t="s">
         <v>23</v>
       </c>
       <c r="L8" s="26" t="s">
@@ -2589,18 +2584,18 @@
     </row>
     <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="86"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="82"/>
       <c r="F9" s="24" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
       <c r="L9" s="26" t="s">
         <v>24</v>
       </c>
@@ -2615,22 +2610,22 @@
     </row>
     <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="92" t="s">
+      <c r="B10" s="89"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="79" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="92" t="s">
+      <c r="H10" s="120"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="92" t="s">
+      <c r="K10" s="79" t="s">
         <v>25</v>
       </c>
       <c r="L10" s="26" t="s">
@@ -2647,18 +2642,18 @@
     </row>
     <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="24" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="93"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="95"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
       <c r="L11" s="26" t="s">
         <v>28</v>
       </c>
@@ -2673,18 +2668,18 @@
     </row>
     <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="86"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="24" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="86"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="82"/>
       <c r="L12" s="26" t="s">
         <v>29</v>
       </c>
@@ -2699,20 +2694,20 @@
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="92" t="s">
+      <c r="B13" s="89"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="79" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>31</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="92" t="s">
+      <c r="H13" s="120"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="79" t="s">
         <v>32</v>
       </c>
       <c r="L13" s="26" t="s">
@@ -2729,18 +2724,18 @@
     </row>
     <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="24" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
       <c r="L14" s="26" t="s">
         <v>33</v>
       </c>
@@ -2755,18 +2750,18 @@
     </row>
     <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
       <c r="F15" s="24" t="s">
         <v>34</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
       <c r="L15" s="26" t="s">
         <v>34</v>
       </c>
@@ -2781,26 +2776,26 @@
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="92" t="s">
+      <c r="B16" s="89"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="92" t="s">
+      <c r="E16" s="79" t="s">
         <v>36</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="98" t="s">
+      <c r="H16" s="120"/>
+      <c r="I16" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="85" t="s">
+      <c r="J16" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="K16" s="92" t="s">
+      <c r="K16" s="79" t="s">
         <v>40</v>
       </c>
       <c r="L16" s="26" t="s">
@@ -2817,18 +2812,18 @@
     </row>
     <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
       <c r="F17" s="24" t="s">
         <v>41</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="86"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="82"/>
       <c r="L17" s="26" t="s">
         <v>41</v>
       </c>
@@ -2843,18 +2838,18 @@
     </row>
     <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
       <c r="F18" s="24" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="92" t="s">
+      <c r="H18" s="120"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="79" t="s">
         <v>43</v>
       </c>
       <c r="L18" s="26" t="s">
@@ -2871,18 +2866,18 @@
     </row>
     <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="86"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="82"/>
       <c r="F19" s="24" t="s">
         <v>44</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
       <c r="L19" s="26" t="s">
         <v>44</v>
       </c>
@@ -2897,22 +2892,22 @@
     </row>
     <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="92" t="s">
+      <c r="B20" s="89"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="79" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>46</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="92" t="s">
+      <c r="H20" s="120"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="K20" s="92" t="s">
+      <c r="K20" s="79" t="s">
         <v>45</v>
       </c>
       <c r="L20" s="26" t="s">
@@ -2929,18 +2924,18 @@
     </row>
     <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
       <c r="F21" s="24" t="s">
         <v>48</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
+      <c r="H21" s="120"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
       <c r="L21" s="26" t="s">
         <v>48</v>
       </c>
@@ -2955,18 +2950,18 @@
     </row>
     <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="24" t="s">
         <v>49</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="93"/>
-      <c r="K22" s="93"/>
+      <c r="H22" s="120"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
       <c r="L22" s="26" t="s">
         <v>49</v>
       </c>
@@ -2981,18 +2976,18 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
       <c r="F23" s="24" t="s">
         <v>50</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="93"/>
-      <c r="K23" s="93"/>
+      <c r="H23" s="120"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
       <c r="L23" s="26" t="s">
         <v>50</v>
       </c>
@@ -3007,18 +3002,18 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="86"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="82"/>
       <c r="F24" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="96"/>
-      <c r="J24" s="93"/>
-      <c r="K24" s="86"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="82"/>
       <c r="L24" s="26" t="s">
         <v>51</v>
       </c>
@@ -3033,20 +3028,20 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="92" t="s">
+      <c r="B25" s="89"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="79" t="s">
         <v>52</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>53</v>
       </c>
       <c r="G25" s="2"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="96"/>
-      <c r="J25" s="93"/>
-      <c r="K25" s="92" t="s">
+      <c r="H25" s="120"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="79" t="s">
         <v>52</v>
       </c>
       <c r="L25" s="26" t="s">
@@ -3063,18 +3058,18 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
       <c r="F26" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G26" s="2"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="96"/>
-      <c r="J26" s="93"/>
-      <c r="K26" s="93"/>
+      <c r="H26" s="120"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
       <c r="L26" s="26" t="s">
         <v>54</v>
       </c>
@@ -3089,18 +3084,18 @@
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="86"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="82"/>
       <c r="F27" s="24" t="s">
         <v>55</v>
       </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="96"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="86"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
       <c r="L27" s="26" t="s">
         <v>55</v>
       </c>
@@ -3115,22 +3110,22 @@
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="93"/>
-      <c r="E28" s="92" t="s">
+      <c r="B28" s="89"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="79" t="s">
         <v>56</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>57</v>
       </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="92" t="s">
+      <c r="H28" s="120"/>
+      <c r="I28" s="95"/>
+      <c r="J28" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="K28" s="92" t="s">
+      <c r="K28" s="79" t="s">
         <v>56</v>
       </c>
       <c r="L28" s="26" t="s">
@@ -3147,18 +3142,18 @@
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="93"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
       <c r="F29" s="24" t="s">
         <v>59</v>
       </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="88"/>
-      <c r="I29" s="96"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="93"/>
+      <c r="H29" s="120"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
       <c r="L29" s="26" t="s">
         <v>59</v>
       </c>
@@ -3173,18 +3168,18 @@
     </row>
     <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="86"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="82"/>
       <c r="F30" s="24" t="s">
         <v>60</v>
       </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="96"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="86"/>
+      <c r="H30" s="120"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="82"/>
       <c r="L30" s="26" t="s">
         <v>60</v>
       </c>
@@ -3199,20 +3194,20 @@
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="92" t="s">
+      <c r="B31" s="89"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="79" t="s">
         <v>61</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>62</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="88"/>
-      <c r="I31" s="96"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="92" t="s">
+      <c r="H31" s="120"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="79" t="s">
         <v>61</v>
       </c>
       <c r="L31" s="26" t="s">
@@ -3229,18 +3224,18 @@
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="83"/>
-      <c r="C32" s="93"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="93"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
       <c r="F32" s="24" t="s">
         <v>63</v>
       </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="88"/>
-      <c r="I32" s="96"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
+      <c r="H32" s="120"/>
+      <c r="I32" s="95"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
       <c r="L32" s="26" t="s">
         <v>63</v>
       </c>
@@ -3255,18 +3250,18 @@
     </row>
     <row r="33" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
       <c r="F33" s="27" t="s">
         <v>64</v>
       </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="89"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="100"/>
-      <c r="K33" s="100"/>
+      <c r="H33" s="121"/>
+      <c r="I33" s="87"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="81"/>
       <c r="L33" s="28" t="s">
         <v>64</v>
       </c>
@@ -3281,10 +3276,10 @@
     </row>
     <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="101" t="s">
+      <c r="B34" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="103" t="s">
+      <c r="C34" s="91" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="29" t="s">
@@ -3295,13 +3290,13 @@
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="104" t="s">
+      <c r="H34" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="I34" s="85" t="s">
+      <c r="I34" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="J34" s="107" t="s">
+      <c r="J34" s="101" t="s">
         <v>70</v>
       </c>
       <c r="K34" s="31" t="s">
@@ -3319,9 +3314,9 @@
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="82"/>
-      <c r="C35" s="93"/>
-      <c r="D35" s="109" t="s">
+      <c r="B35" s="108"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="111" t="s">
         <v>72</v>
       </c>
       <c r="E35" s="33" t="s">
@@ -3329,9 +3324,9 @@
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="107"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="96"/>
+      <c r="J35" s="101"/>
       <c r="K35" s="35" t="s">
         <v>74</v>
       </c>
@@ -3349,18 +3344,18 @@
     </row>
     <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
+      <c r="B36" s="108"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
       <c r="E36" s="33" t="s">
         <v>76</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="85"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="111" t="s">
+      <c r="H36" s="92"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="101"/>
+      <c r="K36" s="112" t="s">
         <v>77</v>
       </c>
       <c r="L36" s="37" t="s">
@@ -3377,18 +3372,18 @@
     </row>
     <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
       <c r="E37" s="33" t="s">
         <v>79</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="104"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="107"/>
-      <c r="K37" s="112"/>
+      <c r="H37" s="92"/>
+      <c r="I37" s="96"/>
+      <c r="J37" s="101"/>
+      <c r="K37" s="113"/>
       <c r="L37" s="38" t="s">
         <v>80</v>
       </c>
@@ -3403,8 +3398,8 @@
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="110" t="s">
+      <c r="B38" s="108"/>
+      <c r="C38" s="83" t="s">
         <v>81</v>
       </c>
       <c r="D38" s="33" t="s">
@@ -3413,10 +3408,10 @@
       <c r="E38" s="33"/>
       <c r="F38" s="34"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="104"/>
-      <c r="I38" s="85"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="112"/>
+      <c r="H38" s="92"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="101"/>
+      <c r="K38" s="113"/>
       <c r="L38" s="38" t="s">
         <v>83</v>
       </c>
@@ -3431,18 +3426,18 @@
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="93"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="80"/>
       <c r="D39" s="33" t="s">
         <v>84</v>
       </c>
       <c r="E39" s="33"/>
       <c r="F39" s="34"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="104"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="107"/>
-      <c r="K39" s="113"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="114"/>
       <c r="L39" s="38" t="s">
         <v>85</v>
       </c>
@@ -3457,18 +3452,18 @@
     </row>
     <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="93"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="80"/>
       <c r="D40" s="33" t="s">
         <v>86</v>
       </c>
       <c r="E40" s="33"/>
       <c r="F40" s="34"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="104"/>
-      <c r="I40" s="85"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="85" t="s">
+      <c r="H40" s="92"/>
+      <c r="I40" s="96"/>
+      <c r="J40" s="101"/>
+      <c r="K40" s="96" t="s">
         <v>87</v>
       </c>
       <c r="L40" s="39" t="s">
@@ -3485,18 +3480,18 @@
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="86"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="82"/>
       <c r="D41" s="33" t="s">
         <v>89</v>
       </c>
       <c r="E41" s="33"/>
       <c r="F41" s="34"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="104"/>
-      <c r="I41" s="85"/>
-      <c r="J41" s="108"/>
-      <c r="K41" s="86"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="96"/>
+      <c r="J41" s="102"/>
+      <c r="K41" s="82"/>
       <c r="L41" s="26" t="s">
         <v>90</v>
       </c>
@@ -3511,11 +3506,11 @@
     </row>
     <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="82"/>
-      <c r="C42" s="110" t="s">
+      <c r="B42" s="108"/>
+      <c r="C42" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="110" t="s">
+      <c r="D42" s="83" t="s">
         <v>92</v>
       </c>
       <c r="E42" s="33" t="s">
@@ -3523,8 +3518,8 @@
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="104"/>
-      <c r="I42" s="85"/>
+      <c r="H42" s="92"/>
+      <c r="I42" s="96"/>
       <c r="J42" s="40" t="s">
         <v>94</v>
       </c>
@@ -3543,22 +3538,22 @@
     </row>
     <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" s="82"/>
-      <c r="C43" s="93"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="110" t="s">
+      <c r="B43" s="108"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="83" t="s">
         <v>96</v>
       </c>
       <c r="F43" s="34" t="s">
         <v>97</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="H43" s="104"/>
-      <c r="I43" s="85"/>
-      <c r="J43" s="114" t="s">
+      <c r="H43" s="92"/>
+      <c r="I43" s="96"/>
+      <c r="J43" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="K43" s="95" t="s">
+      <c r="K43" s="84" t="s">
         <v>99</v>
       </c>
       <c r="L43" s="43" t="s">
@@ -3575,18 +3570,18 @@
     </row>
     <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="82"/>
-      <c r="C44" s="93"/>
-      <c r="D44" s="93"/>
-      <c r="E44" s="93"/>
+      <c r="B44" s="108"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="80"/>
       <c r="F44" s="34" t="s">
         <v>101</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="104"/>
-      <c r="I44" s="85"/>
-      <c r="J44" s="96"/>
-      <c r="K44" s="96"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="96"/>
+      <c r="J44" s="95"/>
+      <c r="K44" s="95"/>
       <c r="L44" s="37" t="s">
         <v>102</v>
       </c>
@@ -3601,18 +3596,18 @@
     </row>
     <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="93"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="93"/>
+      <c r="B45" s="108"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="80"/>
       <c r="F45" s="44" t="s">
         <v>103</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="H45" s="104"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="96"/>
-      <c r="K45" s="96"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="95"/>
+      <c r="K45" s="95"/>
       <c r="L45" s="43" t="s">
         <v>104</v>
       </c>
@@ -3627,18 +3622,18 @@
     </row>
     <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="93"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="80"/>
       <c r="D46" s="45" t="s">
         <v>105</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="47"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="104"/>
-      <c r="I46" s="106"/>
-      <c r="J46" s="97"/>
-      <c r="K46" s="97"/>
+      <c r="H46" s="92"/>
+      <c r="I46" s="104"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="85"/>
       <c r="L46" s="43" t="s">
         <v>106</v>
       </c>
@@ -3653,19 +3648,19 @@
     </row>
     <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="86"/>
+      <c r="B47" s="108"/>
+      <c r="C47" s="82"/>
       <c r="D47" s="48" t="s">
         <v>107</v>
       </c>
       <c r="E47" s="49"/>
       <c r="F47" s="50"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="104"/>
-      <c r="I47" s="92" t="s">
+      <c r="H47" s="92"/>
+      <c r="I47" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="J47" s="115" t="s">
+      <c r="J47" s="100" t="s">
         <v>109</v>
       </c>
       <c r="K47" s="51" t="s">
@@ -3685,11 +3680,11 @@
     </row>
     <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="82"/>
-      <c r="C48" s="110" t="s">
+      <c r="B48" s="108"/>
+      <c r="C48" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="109" t="s">
+      <c r="D48" s="111" t="s">
         <v>112</v>
       </c>
       <c r="E48" s="53" t="s">
@@ -3697,9 +3692,9 @@
       </c>
       <c r="F48" s="54"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="104"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="107"/>
+      <c r="H48" s="92"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="101"/>
       <c r="K48" s="55" t="s">
         <v>114</v>
       </c>
@@ -3715,9 +3710,9 @@
     </row>
     <row r="49" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="82"/>
-      <c r="C49" s="93"/>
-      <c r="D49" s="93"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
       <c r="E49" s="33" t="s">
         <v>115</v>
       </c>
@@ -3725,10 +3720,10 @@
         <v>116</v>
       </c>
       <c r="G49" s="2"/>
-      <c r="H49" s="104"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="107"/>
-      <c r="K49" s="116" t="s">
+      <c r="H49" s="92"/>
+      <c r="I49" s="96"/>
+      <c r="J49" s="101"/>
+      <c r="K49" s="103" t="s">
         <v>117</v>
       </c>
       <c r="L49" s="26" t="s">
@@ -3745,18 +3740,18 @@
     </row>
     <row r="50" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="82"/>
-      <c r="C50" s="93"/>
-      <c r="D50" s="86"/>
+      <c r="B50" s="108"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="82"/>
       <c r="E50" s="33" t="s">
         <v>119</v>
       </c>
       <c r="F50" s="34"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="104"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="107"/>
-      <c r="K50" s="85"/>
+      <c r="H50" s="92"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="101"/>
+      <c r="K50" s="96"/>
       <c r="L50" s="56" t="s">
         <v>120</v>
       </c>
@@ -3771,9 +3766,9 @@
     </row>
     <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="B51" s="82"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="110" t="s">
+      <c r="B51" s="108"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="83" t="s">
         <v>121</v>
       </c>
       <c r="E51" s="33" t="s">
@@ -3781,10 +3776,10 @@
       </c>
       <c r="F51" s="34"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="104"/>
-      <c r="I51" s="85"/>
-      <c r="J51" s="107"/>
-      <c r="K51" s="85"/>
+      <c r="H51" s="92"/>
+      <c r="I51" s="96"/>
+      <c r="J51" s="101"/>
+      <c r="K51" s="96"/>
       <c r="L51" s="26" t="s">
         <v>123</v>
       </c>
@@ -3799,18 +3794,18 @@
     </row>
     <row r="52" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="B52" s="82"/>
-      <c r="C52" s="86"/>
-      <c r="D52" s="86"/>
+      <c r="B52" s="108"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
       <c r="E52" s="33" t="s">
         <v>124</v>
       </c>
       <c r="F52" s="34"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="104"/>
-      <c r="I52" s="85"/>
-      <c r="J52" s="107"/>
-      <c r="K52" s="106"/>
+      <c r="H52" s="92"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="101"/>
+      <c r="K52" s="104"/>
       <c r="L52" s="26" t="s">
         <v>125</v>
       </c>
@@ -3825,11 +3820,11 @@
     </row>
     <row r="53" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
-      <c r="B53" s="82"/>
-      <c r="C53" s="110" t="s">
+      <c r="B53" s="108"/>
+      <c r="C53" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="D53" s="110" t="s">
+      <c r="D53" s="83" t="s">
         <v>127</v>
       </c>
       <c r="E53" s="33" t="s">
@@ -3839,10 +3834,10 @@
         <v>129</v>
       </c>
       <c r="G53" s="2"/>
-      <c r="H53" s="104"/>
-      <c r="I53" s="85"/>
-      <c r="J53" s="107"/>
-      <c r="K53" s="85" t="s">
+      <c r="H53" s="92"/>
+      <c r="I53" s="96"/>
+      <c r="J53" s="101"/>
+      <c r="K53" s="96" t="s">
         <v>130</v>
       </c>
       <c r="L53" s="26" t="s">
@@ -3859,18 +3854,18 @@
     </row>
     <row r="54" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="B54" s="82"/>
-      <c r="C54" s="93"/>
-      <c r="D54" s="93"/>
+      <c r="B54" s="108"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
       <c r="E54" s="33" t="s">
         <v>131</v>
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="104"/>
-      <c r="I54" s="85"/>
-      <c r="J54" s="107"/>
-      <c r="K54" s="85"/>
+      <c r="H54" s="92"/>
+      <c r="I54" s="96"/>
+      <c r="J54" s="101"/>
+      <c r="K54" s="96"/>
       <c r="L54" s="26" t="s">
         <v>101</v>
       </c>
@@ -3885,18 +3880,18 @@
     </row>
     <row r="55" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="B55" s="82"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="93"/>
+      <c r="B55" s="108"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
       <c r="E55" s="33" t="s">
         <v>132</v>
       </c>
       <c r="F55" s="34"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="104"/>
-      <c r="I55" s="85"/>
-      <c r="J55" s="107"/>
-      <c r="K55" s="117" t="s">
+      <c r="H55" s="92"/>
+      <c r="I55" s="96"/>
+      <c r="J55" s="101"/>
+      <c r="K55" s="97" t="s">
         <v>133</v>
       </c>
       <c r="L55" s="38" t="s">
@@ -3913,18 +3908,18 @@
     </row>
     <row r="56" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="B56" s="82"/>
-      <c r="C56" s="93"/>
-      <c r="D56" s="86"/>
+      <c r="B56" s="108"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="82"/>
       <c r="E56" s="33" t="s">
         <v>135</v>
       </c>
       <c r="F56" s="34"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="104"/>
-      <c r="I56" s="106"/>
-      <c r="J56" s="108"/>
-      <c r="K56" s="118"/>
+      <c r="H56" s="92"/>
+      <c r="I56" s="104"/>
+      <c r="J56" s="102"/>
+      <c r="K56" s="98"/>
       <c r="L56" s="57" t="s">
         <v>136</v>
       </c>
@@ -3939,9 +3934,9 @@
     </row>
     <row r="57" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="B57" s="82"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="110" t="s">
+      <c r="B57" s="108"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="83" t="s">
         <v>117</v>
       </c>
       <c r="E57" s="33" t="s">
@@ -3951,11 +3946,11 @@
         <v>138</v>
       </c>
       <c r="G57" s="2"/>
-      <c r="H57" s="104"/>
-      <c r="I57" s="92" t="s">
+      <c r="H57" s="92"/>
+      <c r="I57" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="J57" s="115" t="s">
+      <c r="J57" s="100" t="s">
         <v>140</v>
       </c>
       <c r="K57" s="58" t="s">
@@ -3975,17 +3970,17 @@
     </row>
     <row r="58" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="B58" s="82"/>
-      <c r="C58" s="93"/>
-      <c r="D58" s="93"/>
+      <c r="B58" s="108"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
       <c r="E58" s="33" t="s">
         <v>142</v>
       </c>
       <c r="F58" s="34"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="104"/>
-      <c r="I58" s="85"/>
-      <c r="J58" s="107"/>
+      <c r="H58" s="92"/>
+      <c r="I58" s="96"/>
+      <c r="J58" s="101"/>
       <c r="K58" s="58" t="s">
         <v>86</v>
       </c>
@@ -4003,18 +3998,18 @@
     </row>
     <row r="59" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
+      <c r="B59" s="108"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="80"/>
       <c r="E59" s="33" t="s">
         <v>123</v>
       </c>
       <c r="F59" s="34"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="104"/>
-      <c r="I59" s="85"/>
-      <c r="J59" s="107"/>
-      <c r="K59" s="116" t="s">
+      <c r="H59" s="92"/>
+      <c r="I59" s="96"/>
+      <c r="J59" s="101"/>
+      <c r="K59" s="103" t="s">
         <v>144</v>
       </c>
       <c r="L59" s="25" t="s">
@@ -4031,18 +4026,18 @@
     </row>
     <row r="60" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
-      <c r="B60" s="82"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="86"/>
+      <c r="B60" s="108"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="82"/>
       <c r="E60" s="33" t="s">
         <v>125</v>
       </c>
       <c r="F60" s="34"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="104"/>
-      <c r="I60" s="85"/>
-      <c r="J60" s="107"/>
-      <c r="K60" s="85"/>
+      <c r="H60" s="92"/>
+      <c r="I60" s="96"/>
+      <c r="J60" s="101"/>
+      <c r="K60" s="96"/>
       <c r="L60" s="56" t="s">
         <v>146</v>
       </c>
@@ -4057,9 +4052,9 @@
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="82"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="110" t="s">
+      <c r="B61" s="108"/>
+      <c r="C61" s="80"/>
+      <c r="D61" s="83" t="s">
         <v>144</v>
       </c>
       <c r="E61" s="33" t="s">
@@ -4069,10 +4064,10 @@
         <v>148</v>
       </c>
       <c r="G61" s="2"/>
-      <c r="H61" s="104"/>
-      <c r="I61" s="85"/>
-      <c r="J61" s="107"/>
-      <c r="K61" s="85"/>
+      <c r="H61" s="92"/>
+      <c r="I61" s="96"/>
+      <c r="J61" s="101"/>
+      <c r="K61" s="96"/>
       <c r="L61" s="26" t="s">
         <v>149</v>
       </c>
@@ -4087,18 +4082,18 @@
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
+      <c r="B62" s="108"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="80"/>
       <c r="E62" s="33" t="s">
         <v>146</v>
       </c>
       <c r="F62" s="34"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="104"/>
-      <c r="I62" s="85"/>
-      <c r="J62" s="107"/>
-      <c r="K62" s="106"/>
+      <c r="H62" s="92"/>
+      <c r="I62" s="96"/>
+      <c r="J62" s="101"/>
+      <c r="K62" s="104"/>
       <c r="L62" s="26" t="s">
         <v>150</v>
       </c>
@@ -4113,17 +4108,17 @@
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="B63" s="82"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
+      <c r="B63" s="108"/>
+      <c r="C63" s="80"/>
+      <c r="D63" s="80"/>
       <c r="E63" s="33" t="s">
         <v>149</v>
       </c>
       <c r="F63" s="34"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="104"/>
-      <c r="I63" s="85"/>
-      <c r="J63" s="108"/>
+      <c r="H63" s="92"/>
+      <c r="I63" s="96"/>
+      <c r="J63" s="102"/>
       <c r="K63" s="60" t="s">
         <v>97</v>
       </c>
@@ -4139,20 +4134,20 @@
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="82"/>
-      <c r="C64" s="93"/>
-      <c r="D64" s="86"/>
+      <c r="B64" s="108"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="82"/>
       <c r="E64" s="33" t="s">
         <v>150</v>
       </c>
       <c r="F64" s="34"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="104"/>
-      <c r="I64" s="85"/>
-      <c r="J64" s="92" t="s">
+      <c r="H64" s="92"/>
+      <c r="I64" s="96"/>
+      <c r="J64" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="K64" s="92" t="s">
+      <c r="K64" s="79" t="s">
         <v>152</v>
       </c>
       <c r="L64" s="26" t="s">
@@ -4169,8 +4164,8 @@
     </row>
     <row r="65" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="82"/>
-      <c r="C65" s="86"/>
+      <c r="B65" s="108"/>
+      <c r="C65" s="82"/>
       <c r="D65" s="33" t="s">
         <v>154</v>
       </c>
@@ -4181,10 +4176,10 @@
         <v>156</v>
       </c>
       <c r="G65" s="2"/>
-      <c r="H65" s="104"/>
-      <c r="I65" s="85"/>
-      <c r="J65" s="85"/>
-      <c r="K65" s="86"/>
+      <c r="H65" s="92"/>
+      <c r="I65" s="96"/>
+      <c r="J65" s="96"/>
+      <c r="K65" s="82"/>
       <c r="L65" s="26" t="s">
         <v>157</v>
       </c>
@@ -4199,11 +4194,11 @@
     </row>
     <row r="66" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="B66" s="82"/>
-      <c r="C66" s="110" t="s">
+      <c r="B66" s="108"/>
+      <c r="C66" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="D66" s="110" t="s">
+      <c r="D66" s="83" t="s">
         <v>159</v>
       </c>
       <c r="E66" s="33" t="s">
@@ -4211,10 +4206,10 @@
       </c>
       <c r="F66" s="34"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="104"/>
-      <c r="I66" s="85"/>
-      <c r="J66" s="85"/>
-      <c r="K66" s="92" t="s">
+      <c r="H66" s="92"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="79" t="s">
         <v>67</v>
       </c>
       <c r="L66" s="26" t="s">
@@ -4231,18 +4226,18 @@
     </row>
     <row r="67" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
-      <c r="B67" s="82"/>
-      <c r="C67" s="93"/>
-      <c r="D67" s="93"/>
+      <c r="B67" s="108"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
       <c r="E67" s="33" t="s">
         <v>134</v>
       </c>
       <c r="F67" s="34"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="104"/>
-      <c r="I67" s="85"/>
-      <c r="J67" s="85"/>
-      <c r="K67" s="106"/>
+      <c r="H67" s="92"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="96"/>
+      <c r="K67" s="104"/>
       <c r="L67" s="62" t="s">
         <v>79</v>
       </c>
@@ -4257,17 +4252,17 @@
     </row>
     <row r="68" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
-      <c r="B68" s="82"/>
-      <c r="C68" s="93"/>
-      <c r="D68" s="86"/>
+      <c r="B68" s="108"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="82"/>
       <c r="E68" s="33" t="s">
         <v>153</v>
       </c>
       <c r="F68" s="34"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="104"/>
-      <c r="I68" s="85"/>
-      <c r="J68" s="85"/>
+      <c r="H68" s="92"/>
+      <c r="I68" s="96"/>
+      <c r="J68" s="96"/>
       <c r="K68" s="63" t="s">
         <v>89</v>
       </c>
@@ -4285,9 +4280,9 @@
     </row>
     <row r="69" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
-      <c r="B69" s="82"/>
-      <c r="C69" s="93"/>
-      <c r="D69" s="110" t="s">
+      <c r="B69" s="108"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="83" t="s">
         <v>162</v>
       </c>
       <c r="E69" s="33" t="s">
@@ -4295,10 +4290,10 @@
       </c>
       <c r="F69" s="34"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="104"/>
-      <c r="I69" s="85"/>
-      <c r="J69" s="107"/>
-      <c r="K69" s="117" t="s">
+      <c r="H69" s="92"/>
+      <c r="I69" s="96"/>
+      <c r="J69" s="101"/>
+      <c r="K69" s="97" t="s">
         <v>154</v>
       </c>
       <c r="L69" s="43" t="s">
@@ -4315,18 +4310,18 @@
     </row>
     <row r="70" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-      <c r="B70" s="82"/>
-      <c r="C70" s="93"/>
-      <c r="D70" s="93"/>
+      <c r="B70" s="108"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="80"/>
       <c r="E70" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F70" s="34"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="104"/>
-      <c r="I70" s="85"/>
-      <c r="J70" s="107"/>
-      <c r="K70" s="120"/>
+      <c r="H70" s="92"/>
+      <c r="I70" s="96"/>
+      <c r="J70" s="101"/>
+      <c r="K70" s="105"/>
       <c r="L70" s="38" t="s">
         <v>165</v>
       </c>
@@ -4341,18 +4336,18 @@
     </row>
     <row r="71" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
-      <c r="B71" s="102"/>
-      <c r="C71" s="94"/>
-      <c r="D71" s="94"/>
+      <c r="B71" s="109"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
       <c r="E71" s="64" t="s">
         <v>157</v>
       </c>
       <c r="F71" s="65"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="104"/>
-      <c r="I71" s="85"/>
-      <c r="J71" s="107"/>
-      <c r="K71" s="121"/>
+      <c r="H71" s="92"/>
+      <c r="I71" s="96"/>
+      <c r="J71" s="101"/>
+      <c r="K71" s="106"/>
       <c r="L71" s="38" t="s">
         <v>166</v>
       </c>
@@ -4373,10 +4368,10 @@
       <c r="E72" s="66"/>
       <c r="F72" s="67"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="104"/>
-      <c r="I72" s="85"/>
-      <c r="J72" s="85"/>
-      <c r="K72" s="85" t="s">
+      <c r="H72" s="92"/>
+      <c r="I72" s="96"/>
+      <c r="J72" s="96"/>
+      <c r="K72" s="96" t="s">
         <v>167</v>
       </c>
       <c r="L72" s="26" t="s">
@@ -4399,10 +4394,10 @@
       <c r="E73" s="66"/>
       <c r="F73" s="67"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="104"/>
-      <c r="I73" s="85"/>
-      <c r="J73" s="106"/>
-      <c r="K73" s="86"/>
+      <c r="H73" s="92"/>
+      <c r="I73" s="96"/>
+      <c r="J73" s="104"/>
+      <c r="K73" s="82"/>
       <c r="L73" s="26" t="s">
         <v>169</v>
       </c>
@@ -4423,9 +4418,9 @@
       <c r="E74" s="66"/>
       <c r="F74" s="67"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="104"/>
-      <c r="I74" s="85"/>
-      <c r="J74" s="92" t="s">
+      <c r="H74" s="92"/>
+      <c r="I74" s="96"/>
+      <c r="J74" s="79" t="s">
         <v>170</v>
       </c>
       <c r="K74" s="68" t="s">
@@ -4449,9 +4444,9 @@
       <c r="E75" s="66"/>
       <c r="F75" s="67"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="104"/>
-      <c r="I75" s="85"/>
-      <c r="J75" s="93"/>
+      <c r="H75" s="92"/>
+      <c r="I75" s="96"/>
+      <c r="J75" s="80"/>
       <c r="K75" s="68" t="s">
         <v>105</v>
       </c>
@@ -4473,9 +4468,9 @@
       <c r="E76" s="66"/>
       <c r="F76" s="67"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="104"/>
-      <c r="I76" s="85"/>
-      <c r="J76" s="86"/>
+      <c r="H76" s="92"/>
+      <c r="I76" s="96"/>
+      <c r="J76" s="82"/>
       <c r="K76" s="68" t="s">
         <v>107</v>
       </c>
@@ -4497,12 +4492,12 @@
       <c r="E77" s="66"/>
       <c r="F77" s="67"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="104"/>
-      <c r="I77" s="85"/>
-      <c r="J77" s="92" t="s">
+      <c r="H77" s="92"/>
+      <c r="I77" s="96"/>
+      <c r="J77" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="K77" s="92" t="s">
+      <c r="K77" s="79" t="s">
         <v>112</v>
       </c>
       <c r="L77" s="26" t="s">
@@ -4525,10 +4520,10 @@
       <c r="E78" s="66"/>
       <c r="F78" s="67"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="104"/>
-      <c r="I78" s="85"/>
-      <c r="J78" s="93"/>
-      <c r="K78" s="93"/>
+      <c r="H78" s="92"/>
+      <c r="I78" s="96"/>
+      <c r="J78" s="80"/>
+      <c r="K78" s="80"/>
       <c r="L78" s="26" t="s">
         <v>115</v>
       </c>
@@ -4549,10 +4544,10 @@
       <c r="E79" s="66"/>
       <c r="F79" s="67"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="104"/>
-      <c r="I79" s="85"/>
-      <c r="J79" s="93"/>
-      <c r="K79" s="86"/>
+      <c r="H79" s="92"/>
+      <c r="I79" s="96"/>
+      <c r="J79" s="80"/>
+      <c r="K79" s="82"/>
       <c r="L79" s="26" t="s">
         <v>119</v>
       </c>
@@ -4573,10 +4568,10 @@
       <c r="E80" s="66"/>
       <c r="F80" s="67"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="104"/>
-      <c r="I80" s="85"/>
-      <c r="J80" s="93"/>
-      <c r="K80" s="92" t="s">
+      <c r="H80" s="92"/>
+      <c r="I80" s="96"/>
+      <c r="J80" s="80"/>
+      <c r="K80" s="79" t="s">
         <v>121</v>
       </c>
       <c r="L80" s="26" t="s">
@@ -4599,10 +4594,10 @@
       <c r="E81" s="66"/>
       <c r="F81" s="67"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="105"/>
-      <c r="I81" s="119"/>
-      <c r="J81" s="100"/>
-      <c r="K81" s="100"/>
+      <c r="H81" s="110"/>
+      <c r="I81" s="99"/>
+      <c r="J81" s="81"/>
+      <c r="K81" s="81"/>
       <c r="L81" s="28" t="s">
         <v>124</v>
       </c>
@@ -4617,10 +4612,10 @@
     </row>
     <row r="82" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
-      <c r="B82" s="101" t="s">
+      <c r="B82" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="C82" s="103" t="s">
+      <c r="C82" s="91" t="s">
         <v>173</v>
       </c>
       <c r="D82" s="29" t="s">
@@ -4629,10 +4624,10 @@
       <c r="E82" s="29"/>
       <c r="F82" s="30"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="104" t="s">
+      <c r="H82" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I82" s="95" t="s">
+      <c r="I82" s="84" t="s">
         <v>175</v>
       </c>
       <c r="J82" s="70" t="s">
@@ -4651,16 +4646,16 @@
     </row>
     <row r="83" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
-      <c r="B83" s="83"/>
-      <c r="C83" s="93"/>
+      <c r="B83" s="89"/>
+      <c r="C83" s="80"/>
       <c r="D83" s="33" t="s">
         <v>177</v>
       </c>
       <c r="E83" s="33"/>
       <c r="F83" s="34"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="122"/>
-      <c r="I83" s="96"/>
+      <c r="H83" s="93"/>
+      <c r="I83" s="95"/>
       <c r="J83" s="68" t="s">
         <v>178</v>
       </c>
@@ -4677,16 +4672,16 @@
     </row>
     <row r="84" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
-      <c r="B84" s="83"/>
-      <c r="C84" s="93"/>
+      <c r="B84" s="89"/>
+      <c r="C84" s="80"/>
       <c r="D84" s="33" t="s">
         <v>179</v>
       </c>
       <c r="E84" s="33"/>
       <c r="F84" s="34"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="122"/>
-      <c r="I84" s="96"/>
+      <c r="H84" s="93"/>
+      <c r="I84" s="95"/>
       <c r="J84" s="68" t="s">
         <v>180</v>
       </c>
@@ -4703,16 +4698,16 @@
     </row>
     <row r="85" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
-      <c r="B85" s="83"/>
-      <c r="C85" s="93"/>
+      <c r="B85" s="89"/>
+      <c r="C85" s="80"/>
       <c r="D85" s="33" t="s">
         <v>181</v>
       </c>
       <c r="E85" s="33"/>
       <c r="F85" s="34"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="122"/>
-      <c r="I85" s="97"/>
+      <c r="H85" s="93"/>
+      <c r="I85" s="85"/>
       <c r="J85" s="71" t="s">
         <v>182</v>
       </c>
@@ -4731,16 +4726,16 @@
     </row>
     <row r="86" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
-      <c r="B86" s="83"/>
-      <c r="C86" s="86"/>
+      <c r="B86" s="89"/>
+      <c r="C86" s="82"/>
       <c r="D86" s="33" t="s">
         <v>184</v>
       </c>
       <c r="E86" s="33"/>
       <c r="F86" s="34"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="122"/>
-      <c r="I86" s="95" t="s">
+      <c r="H86" s="93"/>
+      <c r="I86" s="84" t="s">
         <v>185</v>
       </c>
       <c r="J86" s="71" t="s">
@@ -4761,8 +4756,8 @@
     </row>
     <row r="87" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
-      <c r="B87" s="83"/>
-      <c r="C87" s="110" t="s">
+      <c r="B87" s="89"/>
+      <c r="C87" s="83" t="s">
         <v>188</v>
       </c>
       <c r="D87" s="33" t="s">
@@ -4771,8 +4766,8 @@
       <c r="E87" s="33"/>
       <c r="F87" s="34"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="122"/>
-      <c r="I87" s="96"/>
+      <c r="H87" s="93"/>
+      <c r="I87" s="95"/>
       <c r="J87" s="71" t="s">
         <v>190</v>
       </c>
@@ -4791,16 +4786,16 @@
     </row>
     <row r="88" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
-      <c r="B88" s="83"/>
-      <c r="C88" s="93"/>
+      <c r="B88" s="89"/>
+      <c r="C88" s="80"/>
       <c r="D88" s="33" t="s">
         <v>192</v>
       </c>
       <c r="E88" s="33"/>
       <c r="F88" s="34"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="122"/>
-      <c r="I88" s="96"/>
+      <c r="H88" s="93"/>
+      <c r="I88" s="95"/>
       <c r="J88" s="71" t="s">
         <v>193</v>
       </c>
@@ -4819,16 +4814,16 @@
     </row>
     <row r="89" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
-      <c r="B89" s="83"/>
-      <c r="C89" s="86"/>
+      <c r="B89" s="89"/>
+      <c r="C89" s="82"/>
       <c r="D89" s="33" t="s">
         <v>195</v>
       </c>
       <c r="E89" s="33"/>
       <c r="F89" s="34"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="122"/>
-      <c r="I89" s="97"/>
+      <c r="H89" s="93"/>
+      <c r="I89" s="85"/>
       <c r="J89" s="71" t="s">
         <v>196</v>
       </c>
@@ -4847,8 +4842,8 @@
     </row>
     <row r="90" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
-      <c r="B90" s="83"/>
-      <c r="C90" s="110" t="s">
+      <c r="B90" s="89"/>
+      <c r="C90" s="83" t="s">
         <v>197</v>
       </c>
       <c r="D90" s="33" t="s">
@@ -4857,11 +4852,11 @@
       <c r="E90" s="33"/>
       <c r="F90" s="34"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="122"/>
-      <c r="I90" s="92" t="s">
+      <c r="H90" s="93"/>
+      <c r="I90" s="79" t="s">
         <v>199</v>
       </c>
-      <c r="J90" s="95" t="s">
+      <c r="J90" s="84" t="s">
         <v>200</v>
       </c>
       <c r="K90" s="68" t="s">
@@ -4879,17 +4874,17 @@
     </row>
     <row r="91" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
-      <c r="B91" s="83"/>
-      <c r="C91" s="93"/>
+      <c r="B91" s="89"/>
+      <c r="C91" s="80"/>
       <c r="D91" s="33" t="s">
         <v>202</v>
       </c>
       <c r="E91" s="33"/>
       <c r="F91" s="34"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="122"/>
-      <c r="I91" s="93"/>
-      <c r="J91" s="97"/>
+      <c r="H91" s="93"/>
+      <c r="I91" s="80"/>
+      <c r="J91" s="85"/>
       <c r="K91" s="68" t="s">
         <v>203</v>
       </c>
@@ -4905,17 +4900,17 @@
     </row>
     <row r="92" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
-      <c r="B92" s="83"/>
-      <c r="C92" s="86"/>
+      <c r="B92" s="89"/>
+      <c r="C92" s="82"/>
       <c r="D92" s="33" t="s">
         <v>204</v>
       </c>
       <c r="E92" s="33"/>
       <c r="F92" s="34"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="122"/>
-      <c r="I92" s="93"/>
-      <c r="J92" s="95" t="s">
+      <c r="H92" s="93"/>
+      <c r="I92" s="80"/>
+      <c r="J92" s="84" t="s">
         <v>205</v>
       </c>
       <c r="K92" s="68" t="s">
@@ -4933,8 +4928,8 @@
     </row>
     <row r="93" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
-      <c r="B93" s="83"/>
-      <c r="C93" s="110" t="s">
+      <c r="B93" s="89"/>
+      <c r="C93" s="83" t="s">
         <v>207</v>
       </c>
       <c r="D93" s="33" t="s">
@@ -4943,9 +4938,9 @@
       <c r="E93" s="33"/>
       <c r="F93" s="34"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="122"/>
-      <c r="I93" s="93"/>
-      <c r="J93" s="97"/>
+      <c r="H93" s="93"/>
+      <c r="I93" s="80"/>
+      <c r="J93" s="85"/>
       <c r="K93" s="68" t="s">
         <v>209</v>
       </c>
@@ -4961,17 +4956,17 @@
     </row>
     <row r="94" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
-      <c r="B94" s="83"/>
-      <c r="C94" s="93"/>
+      <c r="B94" s="89"/>
+      <c r="C94" s="80"/>
       <c r="D94" s="33" t="s">
         <v>191</v>
       </c>
       <c r="E94" s="33"/>
       <c r="F94" s="34"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="122"/>
-      <c r="I94" s="93"/>
-      <c r="J94" s="95" t="s">
+      <c r="H94" s="93"/>
+      <c r="I94" s="80"/>
+      <c r="J94" s="84" t="s">
         <v>210</v>
       </c>
       <c r="K94" s="68" t="s">
@@ -4989,17 +4984,17 @@
     </row>
     <row r="95" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
-      <c r="B95" s="83"/>
-      <c r="C95" s="86"/>
+      <c r="B95" s="89"/>
+      <c r="C95" s="82"/>
       <c r="D95" s="33" t="s">
         <v>206</v>
       </c>
       <c r="E95" s="33"/>
       <c r="F95" s="34"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="122"/>
-      <c r="I95" s="93"/>
-      <c r="J95" s="97"/>
+      <c r="H95" s="93"/>
+      <c r="I95" s="80"/>
+      <c r="J95" s="85"/>
       <c r="K95" s="68" t="s">
         <v>212</v>
       </c>
@@ -5015,8 +5010,8 @@
     </row>
     <row r="96" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
-      <c r="B96" s="83"/>
-      <c r="C96" s="110" t="s">
+      <c r="B96" s="89"/>
+      <c r="C96" s="83" t="s">
         <v>213</v>
       </c>
       <c r="D96" s="33" t="s">
@@ -5025,9 +5020,9 @@
       <c r="E96" s="33"/>
       <c r="F96" s="34"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="122"/>
-      <c r="I96" s="93"/>
-      <c r="J96" s="95" t="s">
+      <c r="H96" s="93"/>
+      <c r="I96" s="80"/>
+      <c r="J96" s="84" t="s">
         <v>215</v>
       </c>
       <c r="K96" s="68" t="s">
@@ -5045,17 +5040,17 @@
     </row>
     <row r="97" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
-      <c r="B97" s="84"/>
-      <c r="C97" s="94"/>
+      <c r="B97" s="90"/>
+      <c r="C97" s="86"/>
       <c r="D97" s="64" t="s">
         <v>217</v>
       </c>
       <c r="E97" s="64"/>
       <c r="F97" s="65"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="123"/>
-      <c r="I97" s="100"/>
-      <c r="J97" s="99"/>
+      <c r="H97" s="94"/>
+      <c r="I97" s="81"/>
+      <c r="J97" s="87"/>
       <c r="K97" s="72" t="s">
         <v>218</v>
       </c>
@@ -13387,23 +13382,62 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="J77:J81"/>
-    <mergeCell ref="K77:K79"/>
-    <mergeCell ref="K80:K81"/>
-    <mergeCell ref="C87:C89"/>
-    <mergeCell ref="C90:C92"/>
-    <mergeCell ref="I90:I97"/>
-    <mergeCell ref="J90:J91"/>
-    <mergeCell ref="J92:J93"/>
-    <mergeCell ref="C93:C95"/>
-    <mergeCell ref="J94:J95"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="J96:J97"/>
-    <mergeCell ref="B82:B97"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="H82:H97"/>
-    <mergeCell ref="I82:I85"/>
-    <mergeCell ref="I86:I89"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="B3:B33"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="H3:H33"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="C6:C33"/>
+    <mergeCell ref="D6:D15"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="I6:I15"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="D16:D33"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="I16:I33"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="J20:J27"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="J28:J33"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="B34:B71"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="H34:H81"/>
+    <mergeCell ref="I34:I46"/>
+    <mergeCell ref="J34:J41"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="C48:C52"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="J64:J73"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="J43:J46"/>
+    <mergeCell ref="K43:K46"/>
+    <mergeCell ref="I47:I56"/>
+    <mergeCell ref="J47:J56"/>
+    <mergeCell ref="K49:K52"/>
+    <mergeCell ref="D51:D52"/>
     <mergeCell ref="C53:C65"/>
     <mergeCell ref="D53:D56"/>
     <mergeCell ref="K53:K54"/>
@@ -13420,62 +13454,23 @@
     <mergeCell ref="K69:K71"/>
     <mergeCell ref="K72:K73"/>
     <mergeCell ref="J74:J76"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="J43:J46"/>
-    <mergeCell ref="K43:K46"/>
-    <mergeCell ref="I47:I56"/>
-    <mergeCell ref="J47:J56"/>
-    <mergeCell ref="K49:K52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="B34:B71"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="H34:H81"/>
-    <mergeCell ref="I34:I46"/>
-    <mergeCell ref="J34:J41"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="J64:J73"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="D16:D33"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="I16:I33"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="J20:J27"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="J28:J33"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="B3:B33"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="H3:H33"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="C6:C33"/>
-    <mergeCell ref="D6:D15"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="I6:I15"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="B82:B97"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="H82:H97"/>
+    <mergeCell ref="I82:I85"/>
+    <mergeCell ref="I86:I89"/>
+    <mergeCell ref="J77:J81"/>
+    <mergeCell ref="K77:K79"/>
+    <mergeCell ref="K80:K81"/>
+    <mergeCell ref="C87:C89"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="I90:I97"/>
+    <mergeCell ref="J90:J91"/>
+    <mergeCell ref="J92:J93"/>
+    <mergeCell ref="C93:C95"/>
+    <mergeCell ref="J94:J95"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="J96:J97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>